<commit_message>
- added time to date for naming output files - added option to include/exclude report in configuration file - othe rminor changes
</commit_message>
<xml_diff>
--- a/Configuration/SCANClim_Configuration.xlsx
+++ b/Configuration/SCANClim_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efsa815-my.sharepoint.com/personal/andrea_maiorano_efsa_europa_eu/Documents/03_PLH/Projects/SCANClim/Configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{D259647B-9840-4862-8C82-36CF1E016DD8}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBF8C3E1-4238-43B5-91A3-BD3F91E97EB3}"/>
   <bookViews>
-    <workbookView xWindow="-20617" yWindow="-4200" windowWidth="20715" windowHeight="13875" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Present, no details</t>
   </si>
@@ -198,7 +198,10 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Amyelois transitella</t>
+    <t>Xanthomonas campestris pv viticola</t>
+  </si>
+  <si>
+    <t>Print html report</t>
   </si>
 </sst>
 </file>
@@ -660,14 +663,14 @@
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.28515625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="26.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.265625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -675,10 +678,10 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -686,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -694,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
@@ -702,7 +705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
@@ -710,7 +713,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -718,7 +721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
@@ -726,7 +729,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
@@ -751,22 +754,22 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -782,22 +785,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="42.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -816,34 +819,34 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="28.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -861,27 +864,27 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -893,20 +896,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="26.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -914,7 +917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -922,7 +925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>38</v>
       </c>
@@ -930,7 +933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
@@ -938,7 +941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
@@ -946,12 +949,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +975,7 @@
           <x14:formula1>
             <xm:f>tech!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B2 B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{482D41D3-29EE-49D4-85AA-B3E82588417B}">
           <x14:formula1>
@@ -992,12 +1003,12 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1005,7 +1016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1013,7 +1024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1021,52 +1032,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
- Save GIS layers - Modified name of Supporting Information folder to Documentation - included a script to map also uncertain points/polygons (not run authomatically)
</commit_message>
<xml_diff>
--- a/Configuration/SCANClim_Configuration.xlsx
+++ b/Configuration/SCANClim_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efsa815-my.sharepoint.com/personal/andrea_maiorano_efsa_europa_eu/Documents/03_PLH/Projects/SCANClim/Configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBF8C3E1-4238-43B5-91A3-BD3F91E97EB3}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E7AFD47-FDE8-4D9C-8DA0-C10480434F96}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32724" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>Present, no details</t>
   </si>
@@ -198,10 +198,13 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Xanthomonas campestris pv viticola</t>
-  </si>
-  <si>
     <t>Print html report</t>
+  </si>
+  <si>
+    <t>Save GIS layers</t>
+  </si>
+  <si>
+    <t>Amyelois transitella</t>
   </si>
 </sst>
 </file>
@@ -784,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -802,7 +805,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -896,9 +899,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -959,9 +962,17 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -975,7 +986,7 @@
           <x14:formula1>
             <xm:f>tech!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 B7</xm:sqref>
+          <xm:sqref>B2 B7:B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{482D41D3-29EE-49D4-85AA-B3E82588417B}">
           <x14:formula1>

</xml_diff>

<commit_message>
various updates + documentation including Draft EFSA scientific report
</commit_message>
<xml_diff>
--- a/Configuration/SCANClim_Configuration.xlsx
+++ b/Configuration/SCANClim_Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efsa815-my.sharepoint.com/personal/andrea_maiorano_efsa_europa_eu/Documents/03_PLH/Projects/SCANClim/Configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C7B27C2-E82D-48E5-A737-953679996B09}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7EE46A2-4616-4547-9265-538AA7B46E5F}"/>
   <bookViews>
-    <workbookView xWindow="32724" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Present, no details</t>
   </si>
@@ -111,18 +111,9 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>Ocean</t>
-  </si>
-  <si>
     <t>Climates</t>
   </si>
   <si>
-    <t>Dsb</t>
-  </si>
-  <si>
-    <t>Dsc</t>
-  </si>
-  <si>
     <t>Download EPPO host table</t>
   </si>
   <si>
@@ -204,7 +195,7 @@
     <t>Save GIS layers</t>
   </si>
   <si>
-    <t>Fusarium odoratissimum</t>
+    <t>Agrilus planipennis</t>
   </si>
 </sst>
 </file>
@@ -710,10 +701,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -726,18 +717,18 @@
     </row>
     <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +745,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -764,17 +755,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -805,7 +796,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +810,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -861,10 +852,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -874,22 +865,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -902,7 +878,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -925,12 +901,12 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -946,7 +922,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -954,15 +930,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -970,7 +946,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -1021,7 +997,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -1037,7 +1013,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1045,52 +1021,52 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed explicit call to gis libraries
</commit_message>
<xml_diff>
--- a/Configuration/SCANClim_Configuration.xlsx
+++ b/Configuration/SCANClim_Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://efsa815-my.sharepoint.com/personal/andrea_maiorano_efsa_europa_eu/Documents/03_PLH/Projects/SCANClim/Configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{E12750ED-4831-420B-BCA4-3F041A358C7F}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="13_ncr:1_{DE72D9F3-DF0E-4758-BAD0-039D2D4D3BEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CD81FA2-61F3-41CA-98F5-DD26552E7E7F}"/>
   <bookViews>
-    <workbookView xWindow="32724" yWindow="-108" windowWidth="30936" windowHeight="17496" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32724" yWindow="-108" windowWidth="30936" windowHeight="17496" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Present, no details</t>
   </si>
@@ -201,14 +201,26 @@
     <t>South_America</t>
   </si>
   <si>
-    <t>Spodoptera frugiperda</t>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>Amyelois transitella</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -217,6 +229,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -313,10 +331,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -340,11 +359,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,12 +692,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="4"/>
@@ -784,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -801,8 +822,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
+      <c r="A2" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B4FD27-DD83-404E-B71B-70883D41A962}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -874,6 +895,21 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -883,7 +919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +951,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -947,7 +983,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -955,7 +991,7 @@
         <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>